<commit_message>
Update trade day data.
</commit_message>
<xml_diff>
--- a/king_index/data/pe/水电/hydropower.xlsx
+++ b/king_index/data/pe/水电/hydropower.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\caoxuCarlos.github.io\king_index\data\pe\水电\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068C815F-480A-428B-BD25-B51550D17A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDEE2AD-A177-4029-AC04-71FEB4A93CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30060" windowHeight="16032" xr2:uid="{86E2F928-A712-4BF4-BF27-11E41F7C316D}"/>
   </bookViews>
@@ -24005,7 +24005,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>

</xml_diff>